<commit_message>
Added new XRechnung DocTypes; TICC-243; TICC-244
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v8.4.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v8.4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\peppol-edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7C6942-8418-46B2-A49A-CE2DB5C12275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5AED9D-AA4E-426F-8963-70E9FA299006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23565" yWindow="1065" windowWidth="27135" windowHeight="19170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1473" uniqueCount="542">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -1651,6 +1651,51 @@
     <t>Typo in syntax version
 TICC-135
 TICC-245</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:cen.eu:en16931:2017#compliant#urn:xoev-de:kosit:standard:xrechnung_2.3::2.1</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:cen.eu:en16931:2017#compliant#urn:xoev-de:kosit:standard:xrechnung_2.3::2.1</t>
+  </si>
+  <si>
+    <t>urn:un:unece:uncefact:data:standard:CrossIndustryInvoice:100::CrossIndustryInvoice##urn:cen.eu:en16931:2017#compliant#urn:xoev-de:kosit:standard:xrechnung_2.3::D16B</t>
+  </si>
+  <si>
+    <t>8.4</t>
+  </si>
+  <si>
+    <t>TICC-243</t>
+  </si>
+  <si>
+    <t>XRechnung UBL Invoice V2.3</t>
+  </si>
+  <si>
+    <t>XRechnung UBL CreditNote V2.3</t>
+  </si>
+  <si>
+    <t>XRechnung CII Invoice V2.3</t>
+  </si>
+  <si>
+    <t>XRechnung UBL Invoice V2.3 Extension</t>
+  </si>
+  <si>
+    <t>XRechnung UBL CreditNote V2.3 Extension</t>
+  </si>
+  <si>
+    <t>XRechnung CII Invoice V2.3 Extension</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:cen.eu:en16931:2017#compliant#urn:xoev-de:kosit:standard:xrechnung_2.3#conformant#urn:xoev-de:kosit:extension:xrechnung_2.3::2.1</t>
+  </si>
+  <si>
+    <t>urn:un:unece:uncefact:data:standard:CrossIndustryInvoice:100::CrossIndustryInvoice##urn:cen.eu:en16931:2017#compliant#urn:xoev-de:kosit:standard:xrechnung_2.3#conformant#urn:xoev-de:kosit:extension:xrechnung_2.3::D16B</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:cen.eu:en16931:2017#compliant#urn:xoev-de:kosit:standard:xrechnung_2.3#conformant#urn:xoev-de:kosit:extension:xrechnung_2.3::2.1</t>
+  </si>
+  <si>
+    <t>TICC-244</t>
   </si>
 </sst>
 </file>
@@ -2254,12 +2299,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45987FB-91F4-488D-A9D3-2F3FAED3E07C}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:L190"/>
+  <dimension ref="A1:L196"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H85" sqref="H85"/>
+      <pane ySplit="1" topLeftCell="A177" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A197" sqref="A197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -2317,7 +2361,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="45" hidden="1">
+    <row r="2" spans="1:12" ht="45">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -2350,7 +2394,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="45" hidden="1">
+    <row r="3" spans="1:12" ht="45">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -2383,7 +2427,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="45" hidden="1">
+    <row r="4" spans="1:12" ht="45">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -2416,7 +2460,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="45" hidden="1">
+    <row r="5" spans="1:12" ht="45">
       <c r="A5" s="5" t="s">
         <v>100</v>
       </c>
@@ -2449,7 +2493,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="45" hidden="1">
+    <row r="6" spans="1:12" ht="45">
       <c r="A6" s="5" t="s">
         <v>103</v>
       </c>
@@ -2482,7 +2526,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="45" hidden="1">
+    <row r="7" spans="1:12" ht="45">
       <c r="A7" s="5" t="s">
         <v>103</v>
       </c>
@@ -2515,7 +2559,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="45" hidden="1">
+    <row r="8" spans="1:12" ht="45">
       <c r="A8" s="5" t="s">
         <v>36</v>
       </c>
@@ -2548,7 +2592,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="30" hidden="1">
+    <row r="9" spans="1:12" ht="30">
       <c r="A9" s="4" t="s">
         <v>28</v>
       </c>
@@ -2581,7 +2625,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="45" hidden="1">
+    <row r="10" spans="1:12" ht="45">
       <c r="A10" s="4" t="s">
         <v>353</v>
       </c>
@@ -2617,7 +2661,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="45" hidden="1">
+    <row r="11" spans="1:12" ht="45">
       <c r="A11" s="4" t="s">
         <v>29</v>
       </c>
@@ -2650,7 +2694,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="30" hidden="1">
+    <row r="12" spans="1:12" ht="30">
       <c r="A12" s="4" t="s">
         <v>25</v>
       </c>
@@ -2683,7 +2727,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="45" hidden="1">
+    <row r="13" spans="1:12" ht="45">
       <c r="A13" s="4" t="s">
         <v>26</v>
       </c>
@@ -2716,7 +2760,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="30" hidden="1">
+    <row r="14" spans="1:12" ht="30">
       <c r="A14" s="4" t="s">
         <v>101</v>
       </c>
@@ -2749,7 +2793,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="45" hidden="1">
+    <row r="15" spans="1:12" ht="45">
       <c r="A15" s="4" t="s">
         <v>102</v>
       </c>
@@ -2782,7 +2826,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="30" hidden="1">
+    <row r="16" spans="1:12" ht="30">
       <c r="A16" s="4" t="s">
         <v>101</v>
       </c>
@@ -2815,7 +2859,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="45" hidden="1">
+    <row r="17" spans="1:12" ht="45">
       <c r="A17" s="4" t="s">
         <v>91</v>
       </c>
@@ -2848,7 +2892,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="45" hidden="1">
+    <row r="18" spans="1:12" ht="45">
       <c r="A18" s="4" t="s">
         <v>92</v>
       </c>
@@ -2881,7 +2925,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="30" hidden="1">
+    <row r="19" spans="1:12" ht="30">
       <c r="A19" s="5" t="s">
         <v>96</v>
       </c>
@@ -2914,7 +2958,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="45" hidden="1">
+    <row r="20" spans="1:12" ht="45">
       <c r="A20" s="5" t="s">
         <v>97</v>
       </c>
@@ -2947,7 +2991,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="45" hidden="1">
+    <row r="21" spans="1:12" ht="45">
       <c r="A21" s="5" t="s">
         <v>97</v>
       </c>
@@ -2980,7 +3024,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="30" hidden="1">
+    <row r="22" spans="1:12" ht="30">
       <c r="A22" s="5" t="s">
         <v>98</v>
       </c>
@@ -3013,7 +3057,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="45" hidden="1">
+    <row r="23" spans="1:12" ht="45">
       <c r="A23" s="5" t="s">
         <v>99</v>
       </c>
@@ -3046,7 +3090,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="30" hidden="1">
+    <row r="24" spans="1:12" ht="30">
       <c r="A24" s="5" t="s">
         <v>98</v>
       </c>
@@ -3079,7 +3123,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="45" hidden="1">
+    <row r="25" spans="1:12" ht="45">
       <c r="A25" s="5" t="s">
         <v>34</v>
       </c>
@@ -3109,7 +3153,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="45" hidden="1">
+    <row r="26" spans="1:12" ht="45">
       <c r="A26" s="5" t="s">
         <v>35</v>
       </c>
@@ -3136,7 +3180,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="45" hidden="1">
+    <row r="27" spans="1:12" ht="45">
       <c r="A27" s="5" t="s">
         <v>94</v>
       </c>
@@ -3169,7 +3213,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="45" hidden="1">
+    <row r="28" spans="1:12" ht="45">
       <c r="A28" s="5" t="s">
         <v>350</v>
       </c>
@@ -3205,7 +3249,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="45" hidden="1">
+    <row r="29" spans="1:12" ht="45">
       <c r="A29" s="5" t="s">
         <v>95</v>
       </c>
@@ -3238,7 +3282,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="45" hidden="1">
+    <row r="30" spans="1:12" ht="45">
       <c r="A30" s="5" t="s">
         <v>39</v>
       </c>
@@ -3271,7 +3315,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="45" hidden="1">
+    <row r="31" spans="1:12" ht="45">
       <c r="A31" s="5" t="s">
         <v>40</v>
       </c>
@@ -3304,7 +3348,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="30" hidden="1">
+    <row r="32" spans="1:12" ht="30">
       <c r="A32" s="5" t="s">
         <v>485</v>
       </c>
@@ -3334,7 +3378,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="30" hidden="1">
+    <row r="33" spans="1:12" ht="30">
       <c r="A33" s="5" t="s">
         <v>486</v>
       </c>
@@ -3364,7 +3408,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="45" hidden="1">
+    <row r="34" spans="1:12" ht="45">
       <c r="A34" s="5" t="s">
         <v>93</v>
       </c>
@@ -3391,7 +3435,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="45" hidden="1">
+    <row r="35" spans="1:12" ht="45">
       <c r="A35" s="5" t="s">
         <v>347</v>
       </c>
@@ -3424,7 +3468,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="45" hidden="1">
+    <row r="36" spans="1:12" ht="45">
       <c r="A36" s="5" t="s">
         <v>125</v>
       </c>
@@ -3454,7 +3498,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="30" hidden="1">
+    <row r="37" spans="1:12" ht="30">
       <c r="A37" s="5" t="s">
         <v>487</v>
       </c>
@@ -3484,7 +3528,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="45" hidden="1">
+    <row r="38" spans="1:12" ht="45">
       <c r="A38" s="5" t="s">
         <v>503</v>
       </c>
@@ -3514,7 +3558,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="45" hidden="1">
+    <row r="39" spans="1:12" ht="45">
       <c r="A39" s="5" t="s">
         <v>502</v>
       </c>
@@ -3544,7 +3588,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="45" hidden="1">
+    <row r="40" spans="1:12" ht="45">
       <c r="A40" s="5" t="s">
         <v>501</v>
       </c>
@@ -3574,7 +3618,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="45" hidden="1">
+    <row r="41" spans="1:12" ht="45">
       <c r="A41" s="5" t="s">
         <v>500</v>
       </c>
@@ -3604,7 +3648,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="45" hidden="1">
+    <row r="42" spans="1:12" ht="45">
       <c r="A42" s="5" t="s">
         <v>499</v>
       </c>
@@ -3634,7 +3678,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="45" hidden="1">
+    <row r="43" spans="1:12" ht="45">
       <c r="A43" s="5" t="s">
         <v>498</v>
       </c>
@@ -3772,7 +3816,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="47" spans="1:12" hidden="1">
+    <row r="47" spans="1:12">
       <c r="A47" s="5" t="s">
         <v>61</v>
       </c>
@@ -3802,7 +3846,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="48" spans="1:12" hidden="1">
+    <row r="48" spans="1:12">
       <c r="A48" s="5" t="s">
         <v>62</v>
       </c>
@@ -3832,7 +3876,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="30" hidden="1">
+    <row r="49" spans="1:12" ht="30">
       <c r="A49" s="5" t="s">
         <v>63</v>
       </c>
@@ -3862,7 +3906,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="30" hidden="1">
+    <row r="50" spans="1:12" ht="30">
       <c r="A50" s="5" t="s">
         <v>64</v>
       </c>
@@ -3892,7 +3936,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="30" hidden="1">
+    <row r="51" spans="1:12" ht="30">
       <c r="A51" s="5" t="s">
         <v>475</v>
       </c>
@@ -3925,7 +3969,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="30" hidden="1">
+    <row r="52" spans="1:12" ht="30">
       <c r="A52" s="5" t="s">
         <v>476</v>
       </c>
@@ -3955,7 +3999,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="30" hidden="1">
+    <row r="53" spans="1:12" ht="30">
       <c r="A53" s="5" t="s">
         <v>477</v>
       </c>
@@ -3985,7 +4029,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="45" hidden="1">
+    <row r="54" spans="1:12" ht="45">
       <c r="A54" s="5" t="s">
         <v>478</v>
       </c>
@@ -4018,7 +4062,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="30" hidden="1">
+    <row r="55" spans="1:12" ht="30">
       <c r="A55" s="5" t="s">
         <v>479</v>
       </c>
@@ -4048,7 +4092,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="30" hidden="1">
+    <row r="56" spans="1:12" ht="30">
       <c r="A56" s="5" t="s">
         <v>481</v>
       </c>
@@ -4078,7 +4122,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="30" hidden="1">
+    <row r="57" spans="1:12" ht="30">
       <c r="A57" s="5" t="s">
         <v>480</v>
       </c>
@@ -4108,7 +4152,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="30" hidden="1">
+    <row r="58" spans="1:12" ht="30">
       <c r="A58" s="5" t="s">
         <v>482</v>
       </c>
@@ -4138,7 +4182,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="30" hidden="1">
+    <row r="59" spans="1:12" ht="30">
       <c r="A59" s="5" t="s">
         <v>483</v>
       </c>
@@ -4168,7 +4212,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="30" hidden="1">
+    <row r="60" spans="1:12" ht="30">
       <c r="A60" s="5" t="s">
         <v>484</v>
       </c>
@@ -4198,7 +4242,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="30" hidden="1">
+    <row r="61" spans="1:12" ht="30">
       <c r="A61" s="5" t="s">
         <v>79</v>
       </c>
@@ -4225,7 +4269,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="30" hidden="1">
+    <row r="62" spans="1:12" ht="30">
       <c r="A62" s="5" t="s">
         <v>81</v>
       </c>
@@ -4252,7 +4296,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="30" hidden="1">
+    <row r="63" spans="1:12" ht="30">
       <c r="A63" s="5" t="s">
         <v>488</v>
       </c>
@@ -4282,7 +4326,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="45" hidden="1">
+    <row r="64" spans="1:12" ht="45">
       <c r="A64" s="5" t="s">
         <v>348</v>
       </c>
@@ -4318,7 +4362,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="45" hidden="1">
+    <row r="65" spans="1:12" ht="45">
       <c r="A65" s="5" t="s">
         <v>489</v>
       </c>
@@ -4459,7 +4503,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="30" hidden="1">
+    <row r="69" spans="1:12" ht="30">
       <c r="A69" s="5" t="s">
         <v>107</v>
       </c>
@@ -4489,7 +4533,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="45" hidden="1">
+    <row r="70" spans="1:12" ht="45">
       <c r="A70" s="5" t="s">
         <v>108</v>
       </c>
@@ -4519,7 +4563,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="30" hidden="1">
+    <row r="71" spans="1:12" ht="30">
       <c r="A71" s="5" t="s">
         <v>112</v>
       </c>
@@ -4549,7 +4593,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="45" hidden="1">
+    <row r="72" spans="1:12" ht="45">
       <c r="A72" s="1" t="s">
         <v>490</v>
       </c>
@@ -4582,7 +4626,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="45" hidden="1">
+    <row r="73" spans="1:12" ht="45">
       <c r="A73" s="1" t="s">
         <v>491</v>
       </c>
@@ -4615,7 +4659,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="45" hidden="1">
+    <row r="74" spans="1:12" ht="45">
       <c r="A74" s="5" t="s">
         <v>118</v>
       </c>
@@ -4645,7 +4689,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="45" hidden="1">
+    <row r="75" spans="1:12" ht="45">
       <c r="A75" s="5" t="s">
         <v>119</v>
       </c>
@@ -4675,7 +4719,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="45" hidden="1">
+    <row r="76" spans="1:12" ht="45">
       <c r="A76" s="5" t="s">
         <v>161</v>
       </c>
@@ -4705,7 +4749,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="45" hidden="1">
+    <row r="77" spans="1:12" ht="45">
       <c r="A77" s="5" t="s">
         <v>164</v>
       </c>
@@ -5077,7 +5121,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="88" spans="1:12" ht="45" hidden="1">
+    <row r="88" spans="1:12" ht="45">
       <c r="A88" s="5" t="s">
         <v>183</v>
       </c>
@@ -5107,7 +5151,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="89" spans="1:12" ht="30" hidden="1">
+    <row r="89" spans="1:12" ht="30">
       <c r="A89" s="5" t="s">
         <v>234</v>
       </c>
@@ -5141,7 +5185,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="90" spans="1:12" ht="30" hidden="1">
+    <row r="90" spans="1:12" ht="30">
       <c r="A90" s="5" t="s">
         <v>235</v>
       </c>
@@ -5175,7 +5219,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="91" spans="1:12" ht="30" hidden="1">
+    <row r="91" spans="1:12" ht="30">
       <c r="A91" s="5" t="s">
         <v>236</v>
       </c>
@@ -5209,7 +5253,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="92" spans="1:12" ht="45" hidden="1">
+    <row r="92" spans="1:12" ht="45">
       <c r="A92" s="5" t="s">
         <v>237</v>
       </c>
@@ -5243,7 +5287,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="93" spans="1:12" hidden="1">
+    <row r="93" spans="1:12">
       <c r="A93" s="5" t="s">
         <v>195</v>
       </c>
@@ -5273,7 +5317,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="94" spans="1:12" hidden="1">
+    <row r="94" spans="1:12">
       <c r="A94" s="5" t="s">
         <v>196</v>
       </c>
@@ -5303,7 +5347,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="95" spans="1:12" ht="30" hidden="1">
+    <row r="95" spans="1:12" ht="30">
       <c r="A95" s="5" t="s">
         <v>197</v>
       </c>
@@ -5459,7 +5503,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="100" spans="1:12" ht="30" hidden="1">
+    <row r="100" spans="1:12" ht="30">
       <c r="A100" s="5" t="s">
         <v>222</v>
       </c>
@@ -5489,7 +5533,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="45" hidden="1">
+    <row r="101" spans="1:12" ht="45">
       <c r="A101" s="5" t="s">
         <v>223</v>
       </c>
@@ -5519,7 +5563,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="45" hidden="1">
+    <row r="102" spans="1:12" ht="45">
       <c r="A102" s="9" t="s">
         <v>224</v>
       </c>
@@ -5549,7 +5593,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="103" spans="1:12" hidden="1">
+    <row r="103" spans="1:12">
       <c r="A103" s="5" t="s">
         <v>233</v>
       </c>
@@ -5576,7 +5620,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="104" spans="1:12" ht="30" hidden="1">
+    <row r="104" spans="1:12" ht="30">
       <c r="A104" s="5" t="s">
         <v>184</v>
       </c>
@@ -5606,7 +5650,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="105" spans="1:12" ht="30" hidden="1">
+    <row r="105" spans="1:12" ht="30">
       <c r="A105" s="5" t="s">
         <v>185</v>
       </c>
@@ -5636,7 +5680,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="106" spans="1:12" ht="30" hidden="1">
+    <row r="106" spans="1:12" ht="30">
       <c r="A106" s="5" t="s">
         <v>186</v>
       </c>
@@ -5666,7 +5710,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="107" spans="1:12" ht="45" hidden="1">
+    <row r="107" spans="1:12" ht="45">
       <c r="A107" s="5" t="s">
         <v>187</v>
       </c>
@@ -5696,7 +5740,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="108" spans="1:12" ht="30" hidden="1">
+    <row r="108" spans="1:12" ht="30">
       <c r="A108" s="1" t="s">
         <v>253</v>
       </c>
@@ -5726,7 +5770,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="60" hidden="1">
+    <row r="109" spans="1:12" ht="60">
       <c r="A109" s="1" t="s">
         <v>254</v>
       </c>
@@ -5756,7 +5800,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="110" spans="1:12" ht="60" hidden="1">
+    <row r="110" spans="1:12" ht="60">
       <c r="A110" s="1" t="s">
         <v>255</v>
       </c>
@@ -5786,7 +5830,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="111" spans="1:12" ht="45" hidden="1">
+    <row r="111" spans="1:12" ht="45">
       <c r="A111" s="1" t="s">
         <v>256</v>
       </c>
@@ -5816,7 +5860,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="112" spans="1:12" ht="45" hidden="1">
+    <row r="112" spans="1:12" ht="45">
       <c r="A112" s="1" t="s">
         <v>257</v>
       </c>
@@ -5846,7 +5890,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="113" spans="1:12" ht="45" hidden="1">
+    <row r="113" spans="1:12" ht="45">
       <c r="A113" s="1" t="s">
         <v>258</v>
       </c>
@@ -5876,7 +5920,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="114" spans="1:12" ht="45" hidden="1">
+    <row r="114" spans="1:12" ht="45">
       <c r="A114" s="1" t="s">
         <v>259</v>
       </c>
@@ -5906,7 +5950,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="115" spans="1:12" ht="60" hidden="1">
+    <row r="115" spans="1:12" ht="60">
       <c r="A115" s="1" t="s">
         <v>260</v>
       </c>
@@ -5936,7 +5980,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="116" spans="1:12" ht="45" hidden="1">
+    <row r="116" spans="1:12" ht="45">
       <c r="A116" s="1" t="s">
         <v>261</v>
       </c>
@@ -5966,7 +6010,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="117" spans="1:12" ht="30" hidden="1">
+    <row r="117" spans="1:12" ht="30">
       <c r="A117" s="1" t="s">
         <v>262</v>
       </c>
@@ -5996,7 +6040,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="118" spans="1:12" ht="45" hidden="1">
+    <row r="118" spans="1:12" ht="45">
       <c r="A118" s="1" t="s">
         <v>263</v>
       </c>
@@ -6026,7 +6070,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="119" spans="1:12" ht="45" hidden="1">
+    <row r="119" spans="1:12" ht="45">
       <c r="A119" s="1" t="s">
         <v>264</v>
       </c>
@@ -6056,7 +6100,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="120" spans="1:12" ht="45" hidden="1">
+    <row r="120" spans="1:12" ht="45">
       <c r="A120" s="1" t="s">
         <v>265</v>
       </c>
@@ -6086,7 +6130,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="121" spans="1:12" ht="45" hidden="1">
+    <row r="121" spans="1:12" ht="45">
       <c r="A121" s="1" t="s">
         <v>266</v>
       </c>
@@ -6116,7 +6160,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="122" spans="1:12" ht="30" hidden="1">
+    <row r="122" spans="1:12" ht="30">
       <c r="A122" s="1" t="s">
         <v>267</v>
       </c>
@@ -6146,7 +6190,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="123" spans="1:12" ht="45" hidden="1">
+    <row r="123" spans="1:12" ht="45">
       <c r="A123" s="1" t="s">
         <v>268</v>
       </c>
@@ -6176,7 +6220,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="124" spans="1:12" hidden="1">
+    <row r="124" spans="1:12">
       <c r="A124" s="1" t="s">
         <v>269</v>
       </c>
@@ -6206,7 +6250,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="125" spans="1:12" ht="45" hidden="1">
+    <row r="125" spans="1:12" ht="45">
       <c r="A125" s="1" t="s">
         <v>270</v>
       </c>
@@ -6236,7 +6280,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="126" spans="1:12" ht="45" hidden="1">
+    <row r="126" spans="1:12" ht="45">
       <c r="A126" s="1" t="s">
         <v>271</v>
       </c>
@@ -6266,7 +6310,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="127" spans="1:12" hidden="1">
+    <row r="127" spans="1:12">
       <c r="A127" s="1" t="s">
         <v>272</v>
       </c>
@@ -6296,7 +6340,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="128" spans="1:12" ht="45" hidden="1">
+    <row r="128" spans="1:12" ht="45">
       <c r="A128" s="1" t="s">
         <v>273</v>
       </c>
@@ -6326,7 +6370,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="129" spans="1:12" ht="45" hidden="1">
+    <row r="129" spans="1:12" ht="45">
       <c r="A129" s="1" t="s">
         <v>274</v>
       </c>
@@ -6356,7 +6400,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="130" spans="1:12" hidden="1">
+    <row r="130" spans="1:12">
       <c r="A130" s="5" t="s">
         <v>492</v>
       </c>
@@ -6388,7 +6432,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="131" spans="1:12" ht="30" hidden="1">
+    <row r="131" spans="1:12" ht="30">
       <c r="A131" s="5" t="s">
         <v>493</v>
       </c>
@@ -6420,7 +6464,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="132" spans="1:12" hidden="1">
+    <row r="132" spans="1:12">
       <c r="A132" s="5" t="s">
         <v>494</v>
       </c>
@@ -6452,7 +6496,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="133" spans="1:12" ht="30" hidden="1">
+    <row r="133" spans="1:12" ht="30">
       <c r="A133" s="5" t="s">
         <v>495</v>
       </c>
@@ -6484,7 +6528,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="134" spans="1:12" ht="45" hidden="1">
+    <row r="134" spans="1:12" ht="45">
       <c r="A134" s="5" t="s">
         <v>309</v>
       </c>
@@ -6513,7 +6557,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="135" spans="1:12" ht="45" hidden="1">
+    <row r="135" spans="1:12" ht="45">
       <c r="A135" s="5" t="s">
         <v>310</v>
       </c>
@@ -6542,7 +6586,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="136" spans="1:12" ht="45" hidden="1">
+    <row r="136" spans="1:12" ht="45">
       <c r="A136" s="5" t="s">
         <v>311</v>
       </c>
@@ -6571,7 +6615,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="137" spans="1:12" ht="45" hidden="1">
+    <row r="137" spans="1:12" ht="45">
       <c r="A137" s="5" t="s">
         <v>312</v>
       </c>
@@ -6600,7 +6644,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="138" spans="1:12" ht="45" hidden="1">
+    <row r="138" spans="1:12" ht="45">
       <c r="A138" s="5" t="s">
         <v>313</v>
       </c>
@@ -6629,7 +6673,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="139" spans="1:12" ht="45" hidden="1">
+    <row r="139" spans="1:12" ht="45">
       <c r="A139" s="5" t="s">
         <v>314</v>
       </c>
@@ -6658,7 +6702,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="140" spans="1:12" ht="30" hidden="1">
+    <row r="140" spans="1:12" ht="30">
       <c r="A140" s="5" t="s">
         <v>315</v>
       </c>
@@ -6687,7 +6731,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="141" spans="1:12" ht="45" hidden="1">
+    <row r="141" spans="1:12" ht="45">
       <c r="A141" s="5" t="s">
         <v>316</v>
       </c>
@@ -6716,7 +6760,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="142" spans="1:12" ht="45" hidden="1">
+    <row r="142" spans="1:12" ht="45">
       <c r="A142" s="5" t="s">
         <v>317</v>
       </c>
@@ -6745,7 +6789,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="143" spans="1:12" ht="45" hidden="1">
+    <row r="143" spans="1:12" ht="45">
       <c r="A143" s="5" t="s">
         <v>318</v>
       </c>
@@ -6774,7 +6818,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="144" spans="1:12" ht="45" hidden="1">
+    <row r="144" spans="1:12" ht="45">
       <c r="A144" s="5" t="s">
         <v>319</v>
       </c>
@@ -6803,7 +6847,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="145" spans="1:12" ht="30" hidden="1">
+    <row r="145" spans="1:12" ht="30">
       <c r="A145" s="5" t="s">
         <v>320</v>
       </c>
@@ -6832,7 +6876,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="146" spans="1:12" ht="45" hidden="1">
+    <row r="146" spans="1:12" ht="45">
       <c r="A146" s="5" t="s">
         <v>321</v>
       </c>
@@ -6861,7 +6905,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="147" spans="1:12" ht="45" hidden="1">
+    <row r="147" spans="1:12" ht="45">
       <c r="A147" s="5" t="s">
         <v>322</v>
       </c>
@@ -7064,7 +7108,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="154" spans="1:12" ht="45" hidden="1">
+    <row r="154" spans="1:12" ht="45">
       <c r="A154" s="5" t="s">
         <v>379</v>
       </c>
@@ -7093,7 +7137,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="155" spans="1:12" ht="45" hidden="1">
+    <row r="155" spans="1:12" ht="45">
       <c r="A155" s="5" t="s">
         <v>380</v>
       </c>
@@ -7122,7 +7166,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="156" spans="1:12" ht="45" hidden="1">
+    <row r="156" spans="1:12" ht="45">
       <c r="A156" s="5" t="s">
         <v>381</v>
       </c>
@@ -7151,7 +7195,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="157" spans="1:12" ht="30" hidden="1">
+    <row r="157" spans="1:12" ht="30">
       <c r="A157" s="5" t="s">
         <v>400</v>
       </c>
@@ -7180,7 +7224,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="158" spans="1:12" ht="30" hidden="1">
+    <row r="158" spans="1:12" ht="30">
       <c r="A158" s="5" t="s">
         <v>401</v>
       </c>
@@ -7209,7 +7253,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="159" spans="1:12" ht="30" hidden="1">
+    <row r="159" spans="1:12" ht="30">
       <c r="A159" s="5" t="s">
         <v>402</v>
       </c>
@@ -7238,7 +7282,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="160" spans="1:12" ht="30" hidden="1">
+    <row r="160" spans="1:12" ht="30">
       <c r="A160" s="5" t="s">
         <v>403</v>
       </c>
@@ -7267,7 +7311,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="161" spans="1:12" hidden="1">
+    <row r="161" spans="1:12">
       <c r="A161" s="5" t="s">
         <v>404</v>
       </c>
@@ -7296,7 +7340,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="162" spans="1:12" ht="30" hidden="1">
+    <row r="162" spans="1:12" ht="30">
       <c r="A162" s="5" t="s">
         <v>405</v>
       </c>
@@ -7325,7 +7369,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="163" spans="1:12" ht="30" hidden="1">
+    <row r="163" spans="1:12" ht="30">
       <c r="A163" s="5" t="s">
         <v>406</v>
       </c>
@@ -7354,7 +7398,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="164" spans="1:12" ht="30" hidden="1">
+    <row r="164" spans="1:12" ht="30">
       <c r="A164" s="5" t="s">
         <v>407</v>
       </c>
@@ -7383,7 +7427,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="165" spans="1:12" ht="30" hidden="1">
+    <row r="165" spans="1:12" ht="30">
       <c r="A165" s="5" t="s">
         <v>408</v>
       </c>
@@ -7412,7 +7456,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="166" spans="1:12" ht="30" hidden="1">
+    <row r="166" spans="1:12" ht="30">
       <c r="A166" s="5" t="s">
         <v>409</v>
       </c>
@@ -7441,7 +7485,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="167" spans="1:12" hidden="1">
+    <row r="167" spans="1:12">
       <c r="A167" s="5" t="s">
         <v>410</v>
       </c>
@@ -7470,7 +7514,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="168" spans="1:12" hidden="1">
+    <row r="168" spans="1:12">
       <c r="A168" s="5" t="s">
         <v>411</v>
       </c>
@@ -7499,7 +7543,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="169" spans="1:12" ht="30" hidden="1">
+    <row r="169" spans="1:12" ht="30">
       <c r="A169" s="5" t="s">
         <v>412</v>
       </c>
@@ -7528,7 +7572,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="170" spans="1:12" ht="30" hidden="1">
+    <row r="170" spans="1:12" ht="30">
       <c r="A170" s="5" t="s">
         <v>413</v>
       </c>
@@ -7557,7 +7601,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="171" spans="1:12" hidden="1">
+    <row r="171" spans="1:12">
       <c r="A171" s="5" t="s">
         <v>416</v>
       </c>
@@ -7586,7 +7630,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="172" spans="1:12" ht="30" hidden="1">
+    <row r="172" spans="1:12" ht="30">
       <c r="A172" s="5" t="s">
         <v>415</v>
       </c>
@@ -7615,7 +7659,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="173" spans="1:12" ht="30" hidden="1">
+    <row r="173" spans="1:12" ht="30">
       <c r="A173" s="5" t="s">
         <v>414</v>
       </c>
@@ -7818,7 +7862,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="180" spans="1:12" hidden="1">
+    <row r="180" spans="1:12">
       <c r="A180" s="5" t="s">
         <v>496</v>
       </c>
@@ -7847,7 +7891,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="181" spans="1:12" ht="30" hidden="1">
+    <row r="181" spans="1:12" ht="30">
       <c r="A181" s="5" t="s">
         <v>497</v>
       </c>
@@ -7876,7 +7920,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="182" spans="1:12" ht="30" hidden="1">
+    <row r="182" spans="1:12" ht="30">
       <c r="A182" s="5" t="s">
         <v>467</v>
       </c>
@@ -7905,7 +7949,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="183" spans="1:12" ht="30" hidden="1">
+    <row r="183" spans="1:12" ht="30">
       <c r="A183" s="5" t="s">
         <v>468</v>
       </c>
@@ -7934,7 +7978,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="184" spans="1:12" ht="30" hidden="1">
+    <row r="184" spans="1:12" ht="30">
       <c r="A184" s="5" t="s">
         <v>469</v>
       </c>
@@ -7963,7 +8007,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="185" spans="1:12" ht="30" hidden="1">
+    <row r="185" spans="1:12" ht="30">
       <c r="A185" s="5" t="s">
         <v>470</v>
       </c>
@@ -7992,7 +8036,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="186" spans="1:12" ht="45" hidden="1">
+    <row r="186" spans="1:12" ht="45">
       <c r="A186" s="5" t="s">
         <v>504</v>
       </c>
@@ -8021,7 +8065,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="187" spans="1:12" hidden="1">
+    <row r="187" spans="1:12">
       <c r="A187" t="s">
         <v>507</v>
       </c>
@@ -8054,7 +8098,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="188" spans="1:12" ht="30" hidden="1">
+    <row r="188" spans="1:12" ht="30">
       <c r="A188" s="5" t="s">
         <v>516</v>
       </c>
@@ -8086,7 +8130,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="189" spans="1:12" ht="30" hidden="1">
+    <row r="189" spans="1:12" ht="30">
       <c r="A189" s="5" t="s">
         <v>517</v>
       </c>
@@ -8118,7 +8162,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="190" spans="1:12" ht="30" hidden="1">
+    <row r="190" spans="1:12" ht="30">
       <c r="A190" s="5" t="s">
         <v>518</v>
       </c>
@@ -8150,45 +8194,182 @@
         <v>512</v>
       </c>
     </row>
+    <row r="191" spans="1:12" ht="30">
+      <c r="A191" s="5" t="s">
+        <v>532</v>
+      </c>
+      <c r="B191" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C191" s="5" t="s">
+        <v>527</v>
+      </c>
+      <c r="D191" s="18" t="s">
+        <v>530</v>
+      </c>
+      <c r="E191" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="H191" s="5" t="s">
+        <v>531</v>
+      </c>
+      <c r="I191" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K191" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="L191" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="192" spans="1:12" ht="30">
+      <c r="A192" s="5" t="s">
+        <v>533</v>
+      </c>
+      <c r="B192" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C192" s="5" t="s">
+        <v>528</v>
+      </c>
+      <c r="D192" s="18" t="s">
+        <v>530</v>
+      </c>
+      <c r="E192" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="H192" s="5" t="s">
+        <v>531</v>
+      </c>
+      <c r="I192" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K192" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="L192" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="193" spans="1:12" ht="30">
+      <c r="A193" s="5" t="s">
+        <v>534</v>
+      </c>
+      <c r="B193" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C193" s="5" t="s">
+        <v>529</v>
+      </c>
+      <c r="D193" s="18" t="s">
+        <v>530</v>
+      </c>
+      <c r="E193" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="H193" s="5" t="s">
+        <v>531</v>
+      </c>
+      <c r="I193" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K193" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="L193" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="194" spans="1:12" ht="30">
+      <c r="A194" s="5" t="s">
+        <v>535</v>
+      </c>
+      <c r="B194" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C194" s="5" t="s">
+        <v>540</v>
+      </c>
+      <c r="D194" s="18" t="s">
+        <v>530</v>
+      </c>
+      <c r="E194" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="H194" s="5" t="s">
+        <v>541</v>
+      </c>
+      <c r="I194" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K194" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="L194" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="195" spans="1:12" ht="45">
+      <c r="A195" s="5" t="s">
+        <v>536</v>
+      </c>
+      <c r="B195" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C195" s="5" t="s">
+        <v>538</v>
+      </c>
+      <c r="D195" s="18" t="s">
+        <v>530</v>
+      </c>
+      <c r="E195" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="H195" s="5" t="s">
+        <v>541</v>
+      </c>
+      <c r="I195" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K195" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="L195" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="196" spans="1:12" ht="45">
+      <c r="A196" s="5" t="s">
+        <v>537</v>
+      </c>
+      <c r="B196" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C196" s="5" t="s">
+        <v>539</v>
+      </c>
+      <c r="D196" s="18" t="s">
+        <v>530</v>
+      </c>
+      <c r="E196" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="H196" s="5" t="s">
+        <v>541</v>
+      </c>
+      <c r="I196" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K196" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="L196" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:L190" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="XRechnung CII Invoice V1.1"/>
-        <filter val="XRechnung CII Invoice V1.2"/>
-        <filter val="XRechnung CII Invoice V1.3"/>
-        <filter val="XRechnung CII Invoice V1.3 Extension"/>
-        <filter val="XRechnung CII Invoice V2.0"/>
-        <filter val="XRechnung CII Invoice V2.0 (invalid)"/>
-        <filter val="XRechnung CII Invoice V2.0 Extension"/>
-        <filter val="XRechnung CII Invoice V2.0 Extension (invalid)"/>
-        <filter val="XRechnung CII Invoice V2.1"/>
-        <filter val="XRechnung CII Invoice V2.1 Extension"/>
-        <filter val="XRechnung CII Invoice V2.2"/>
-        <filter val="XRechnung CII Invoice V2.2 Extension"/>
-        <filter val="XRechnung UBL CreditNote V1.1"/>
-        <filter val="XRechnung UBL CreditNote V1.2"/>
-        <filter val="XRechnung UBL CreditNote V1.3"/>
-        <filter val="XRechnung UBL CreditNote V1.3 Extension"/>
-        <filter val="XRechnung UBL CreditNote V2.0"/>
-        <filter val="XRechnung UBL CreditNote V2.0 Extension"/>
-        <filter val="XRechnung UBL CreditNote V2.1"/>
-        <filter val="XRechnung UBL CreditNote V2.1 Extension"/>
-        <filter val="XRechnung UBL CreditNote V2.2"/>
-        <filter val="XRechnung UBL CreditNote V2.2 Extension"/>
-        <filter val="XRechnung UBL Invoice V1.1"/>
-        <filter val="XRechnung UBL Invoice V1.2"/>
-        <filter val="XRechnung UBL Invoice V1.3"/>
-        <filter val="XRechnung UBL Invoice V1.3 Extension"/>
-        <filter val="XRechnung UBL Invoice V2.0"/>
-        <filter val="XRechnung UBL Invoice V2.0 Extension"/>
-        <filter val="XRechnung UBL Invoice V2.1"/>
-        <filter val="XRechnung UBL Invoice V2.1 Extension"/>
-        <filter val="XRechnung UBL Invoice V2.2"/>
-        <filter val="XRechnung UBL Invoice V2.2 Extension"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:L190" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>